<commit_message>
added more dummy data
</commit_message>
<xml_diff>
--- a/app/DB_init/readings.xlsx
+++ b/app/DB_init/readings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\IOT_Project\app\DB_init\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junyi/Desktop/School/CS462 - IoT Technology &amp; Application/IOT_Project/app/DB_init/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5366C54-D5A4-48F3-A48B-32495C96456C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63AE3AC-612C-BA44-8A12-97966D3A6AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="194">
   <si>
     <t>Before_CBG_Reading</t>
   </si>
@@ -472,16 +472,158 @@
   </si>
   <si>
     <t>2023-04-02 19:15</t>
+  </si>
+  <si>
+    <t>2023-04-03 10:00</t>
+  </si>
+  <si>
+    <t>2023-04-03 18:00</t>
+  </si>
+  <si>
+    <t>2023-04-04 10:00</t>
+  </si>
+  <si>
+    <t>2023-04-04 18:00</t>
+  </si>
+  <si>
+    <t>2023-04-05 10:00</t>
+  </si>
+  <si>
+    <t>2023-04-05 18:00</t>
+  </si>
+  <si>
+    <t>2023-04-06 10:00</t>
+  </si>
+  <si>
+    <t>2023-04-06 18:00</t>
+  </si>
+  <si>
+    <t>2023-04-07 10:00</t>
+  </si>
+  <si>
+    <t>2023-04-07 18:00</t>
+  </si>
+  <si>
+    <t>2023-04-08 10:00</t>
+  </si>
+  <si>
+    <t>2023-04-08 18:00</t>
+  </si>
+  <si>
+    <t>2023-04-09 10:00</t>
+  </si>
+  <si>
+    <t>2023-04-09 18:00</t>
+  </si>
+  <si>
+    <t>2023-04-10 10:00</t>
+  </si>
+  <si>
+    <t>2023-04-03 10:30</t>
+  </si>
+  <si>
+    <t>2023-04-03 18:30</t>
+  </si>
+  <si>
+    <t>2023-04-04 10:30</t>
+  </si>
+  <si>
+    <t>2023-04-04 18:30</t>
+  </si>
+  <si>
+    <t>2023-04-05 10:30</t>
+  </si>
+  <si>
+    <t>2023-04-05 18:30</t>
+  </si>
+  <si>
+    <t>2023-04-06 10:30</t>
+  </si>
+  <si>
+    <t>2023-04-06 18:30</t>
+  </si>
+  <si>
+    <t>2023-04-07 10:30</t>
+  </si>
+  <si>
+    <t>2023-04-07 18:30</t>
+  </si>
+  <si>
+    <t>2023-04-08 10:30</t>
+  </si>
+  <si>
+    <t>2023-04-08 18:30</t>
+  </si>
+  <si>
+    <t>2023-04-09 10:30</t>
+  </si>
+  <si>
+    <t>2023-04-09 18:30</t>
+  </si>
+  <si>
+    <t>2023-04-10 10:30</t>
+  </si>
+  <si>
+    <t>2023-04-03 11:15</t>
+  </si>
+  <si>
+    <t>2023-04-03 19:15</t>
+  </si>
+  <si>
+    <t>2023-04-04 11:15</t>
+  </si>
+  <si>
+    <t>2023-04-04 19:15</t>
+  </si>
+  <si>
+    <t>2023-04-05 11:15</t>
+  </si>
+  <si>
+    <t>2023-04-05 19:15</t>
+  </si>
+  <si>
+    <t>2023-04-06 11:15</t>
+  </si>
+  <si>
+    <t>2023-04-06 19:15</t>
+  </si>
+  <si>
+    <t>2023-04-07 11:15</t>
+  </si>
+  <si>
+    <t>2023-04-07 19:15</t>
+  </si>
+  <si>
+    <t>2023-04-08 11:15</t>
+  </si>
+  <si>
+    <t>2023-04-08 19:15</t>
+  </si>
+  <si>
+    <t>2023-04-09 11:15</t>
+  </si>
+  <si>
+    <t>2023-04-09 19:15</t>
+  </si>
+  <si>
+    <t>2023-04-10 11:15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -507,9 +649,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -790,29 +934,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L57"/>
+  <dimension ref="A1:L69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="M38" sqref="M38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L61" sqref="L61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="24" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -850,7 +994,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>6</v>
       </c>
@@ -888,7 +1032,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>6</v>
       </c>
@@ -926,7 +1070,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>6.2</v>
       </c>
@@ -964,7 +1108,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>6.4</v>
       </c>
@@ -1002,7 +1146,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>6.4</v>
       </c>
@@ -1040,7 +1184,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6.2</v>
       </c>
@@ -1078,7 +1222,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6.3</v>
       </c>
@@ -1116,7 +1260,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>6.2</v>
       </c>
@@ -1154,7 +1298,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6.3</v>
       </c>
@@ -1192,7 +1336,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>6.1</v>
       </c>
@@ -1230,7 +1374,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>6.2</v>
       </c>
@@ -1268,7 +1412,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>6.3</v>
       </c>
@@ -1306,7 +1450,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>6.3</v>
       </c>
@@ -1344,7 +1488,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>6.2</v>
       </c>
@@ -1382,7 +1526,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>6.3</v>
       </c>
@@ -1420,7 +1564,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>6.4</v>
       </c>
@@ -1458,7 +1602,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>6.3</v>
       </c>
@@ -1496,7 +1640,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>6.3</v>
       </c>
@@ -1534,7 +1678,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>6.3</v>
       </c>
@@ -1572,7 +1716,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>6.4</v>
       </c>
@@ -1610,7 +1754,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>6.3</v>
       </c>
@@ -1648,7 +1792,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>6.4</v>
       </c>
@@ -1686,7 +1830,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>6.5</v>
       </c>
@@ -1724,7 +1868,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>6.7</v>
       </c>
@@ -1762,7 +1906,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>6.8</v>
       </c>
@@ -1800,7 +1944,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>6.9</v>
       </c>
@@ -1838,7 +1982,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>6.7</v>
       </c>
@@ -1876,7 +2020,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>6.8</v>
       </c>
@@ -1914,7 +2058,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>6.7</v>
       </c>
@@ -1952,7 +2096,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>6.9</v>
       </c>
@@ -1990,7 +2134,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>6</v>
       </c>
@@ -2028,7 +2172,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>6</v>
       </c>
@@ -2066,7 +2210,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>6.2</v>
       </c>
@@ -2104,7 +2248,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>6.4</v>
       </c>
@@ -2142,7 +2286,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>6.4</v>
       </c>
@@ -2180,7 +2324,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>6.2</v>
       </c>
@@ -2218,7 +2362,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>6.3</v>
       </c>
@@ -2256,7 +2400,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>6.2</v>
       </c>
@@ -2294,7 +2438,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>6.3</v>
       </c>
@@ -2332,7 +2476,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>6.1</v>
       </c>
@@ -2370,7 +2514,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>6.2</v>
       </c>
@@ -2408,7 +2552,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>6.3</v>
       </c>
@@ -2446,7 +2590,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>6.3</v>
       </c>
@@ -2484,7 +2628,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>6.2</v>
       </c>
@@ -2522,41 +2666,701 @@
         <v>148</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C46" s="1"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C47" s="1"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C48" s="1"/>
-    </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C49" s="1"/>
-    </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C50" s="1"/>
-    </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C51" s="1"/>
-    </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C52" s="1"/>
-    </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C53" s="1"/>
-    </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C54" s="1"/>
-    </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C55" s="1"/>
-    </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C56" s="1"/>
-    </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C57" s="1"/>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A46" s="2">
+        <v>6.3</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E46" s="2">
+        <v>80</v>
+      </c>
+      <c r="F46" s="2">
+        <v>20</v>
+      </c>
+      <c r="G46" s="2">
+        <v>4</v>
+      </c>
+      <c r="H46" s="2">
+        <v>3</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="J46" s="2">
+        <v>6.4</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L46" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A47" s="2">
+        <v>6.4</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E47" s="2">
+        <v>266</v>
+      </c>
+      <c r="F47" s="2">
+        <v>30.3</v>
+      </c>
+      <c r="G47" s="2">
+        <v>5.2</v>
+      </c>
+      <c r="H47" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="J47" s="2">
+        <v>6.6</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L47" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A48" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E48" s="2">
+        <v>284.2</v>
+      </c>
+      <c r="F48" s="2">
+        <v>11.5</v>
+      </c>
+      <c r="G48" s="2">
+        <v>0</v>
+      </c>
+      <c r="H48" s="2">
+        <v>2</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="J48" s="2">
+        <v>6.7</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L48" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A49" s="2">
+        <v>6.7</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E49" s="2">
+        <v>266</v>
+      </c>
+      <c r="F49" s="2">
+        <v>30.3</v>
+      </c>
+      <c r="G49" s="2">
+        <v>5.2</v>
+      </c>
+      <c r="H49" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="J49" s="2">
+        <v>7</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L49" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A50" s="2">
+        <v>6.8</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E50" s="2">
+        <v>284.2</v>
+      </c>
+      <c r="F50" s="2">
+        <v>11.5</v>
+      </c>
+      <c r="G50" s="2">
+        <v>0</v>
+      </c>
+      <c r="H50" s="2">
+        <v>2</v>
+      </c>
+      <c r="I50" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="J50" s="2">
+        <v>7</v>
+      </c>
+      <c r="K50" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L50" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A51" s="2">
+        <v>6.9</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E51" s="2">
+        <v>266</v>
+      </c>
+      <c r="F51" s="2">
+        <v>30.3</v>
+      </c>
+      <c r="G51" s="2">
+        <v>5.2</v>
+      </c>
+      <c r="H51" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="J51" s="2">
+        <v>7.2</v>
+      </c>
+      <c r="K51" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L51" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A52" s="2">
+        <v>6.7</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E52" s="2">
+        <v>284.2</v>
+      </c>
+      <c r="F52" s="2">
+        <v>11.5</v>
+      </c>
+      <c r="G52" s="2">
+        <v>0</v>
+      </c>
+      <c r="H52" s="2">
+        <v>2</v>
+      </c>
+      <c r="I52" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="J52" s="2">
+        <v>6.9</v>
+      </c>
+      <c r="K52" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L52" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A53" s="2">
+        <v>6.8</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E53" s="2">
+        <v>248</v>
+      </c>
+      <c r="F53" s="2">
+        <v>51.7</v>
+      </c>
+      <c r="G53" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="H53" s="2">
+        <v>3.23</v>
+      </c>
+      <c r="I53" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="J53" s="2">
+        <v>6.8</v>
+      </c>
+      <c r="K53" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L53" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A54" s="2">
+        <v>6.7</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E54" s="2">
+        <v>284.2</v>
+      </c>
+      <c r="F54" s="2">
+        <v>11.5</v>
+      </c>
+      <c r="G54" s="2">
+        <v>0</v>
+      </c>
+      <c r="H54" s="2">
+        <v>2</v>
+      </c>
+      <c r="I54" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="J54" s="2">
+        <v>6.9</v>
+      </c>
+      <c r="K54" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L54" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A55" s="2">
+        <v>6.9</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E55" s="2">
+        <v>248</v>
+      </c>
+      <c r="F55" s="2">
+        <v>51.7</v>
+      </c>
+      <c r="G55" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="H55" s="2">
+        <v>3.23</v>
+      </c>
+      <c r="I55" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="J55" s="2">
+        <v>7</v>
+      </c>
+      <c r="K55" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L55" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A56" s="2">
+        <v>6</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E56" s="2">
+        <v>80</v>
+      </c>
+      <c r="F56" s="2">
+        <v>20</v>
+      </c>
+      <c r="G56" s="2">
+        <v>4</v>
+      </c>
+      <c r="H56" s="2">
+        <v>3</v>
+      </c>
+      <c r="I56" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="J56" s="2">
+        <v>6.1</v>
+      </c>
+      <c r="K56" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L56" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A57" s="2">
+        <v>6</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E57" s="2">
+        <v>266</v>
+      </c>
+      <c r="F57" s="2">
+        <v>30.3</v>
+      </c>
+      <c r="G57" s="2">
+        <v>5.2</v>
+      </c>
+      <c r="H57" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I57" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="J57" s="2">
+        <v>6.3</v>
+      </c>
+      <c r="K57" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L57" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A58" s="2">
+        <v>6.2</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E58" s="2">
+        <v>284.2</v>
+      </c>
+      <c r="F58" s="2">
+        <v>11.5</v>
+      </c>
+      <c r="G58" s="2">
+        <v>0</v>
+      </c>
+      <c r="H58" s="2">
+        <v>2</v>
+      </c>
+      <c r="I58" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="J58" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="K58" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L58" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A59" s="2">
+        <v>6.4</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E59" s="2">
+        <v>266</v>
+      </c>
+      <c r="F59" s="2">
+        <v>30.3</v>
+      </c>
+      <c r="G59" s="2">
+        <v>5.2</v>
+      </c>
+      <c r="H59" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I59" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J59" s="2">
+        <v>6.7</v>
+      </c>
+      <c r="K59" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L59" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A60" s="2">
+        <v>6.4</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E60" s="2">
+        <v>80</v>
+      </c>
+      <c r="F60" s="2">
+        <v>20</v>
+      </c>
+      <c r="G60" s="2">
+        <v>4</v>
+      </c>
+      <c r="H60" s="2">
+        <v>3</v>
+      </c>
+      <c r="I60" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="J60" s="2">
+        <v>6.4</v>
+      </c>
+      <c r="K60" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L60" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A61" s="2"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="3"/>
+      <c r="J61" s="2"/>
+      <c r="K61" s="2"/>
+      <c r="L61" s="3"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A62" s="2"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
+      <c r="H62" s="2"/>
+      <c r="I62" s="3"/>
+      <c r="J62" s="2"/>
+      <c r="K62" s="2"/>
+      <c r="L62" s="3"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A63" s="2"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2"/>
+      <c r="I63" s="3"/>
+      <c r="J63" s="2"/>
+      <c r="K63" s="2"/>
+      <c r="L63" s="3"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A64" s="2"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+      <c r="H64" s="2"/>
+      <c r="I64" s="3"/>
+      <c r="J64" s="2"/>
+      <c r="K64" s="2"/>
+      <c r="L64" s="3"/>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A65" s="2"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="3"/>
+      <c r="J65" s="2"/>
+      <c r="K65" s="2"/>
+      <c r="L65" s="3"/>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A66" s="2"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2"/>
+      <c r="I66" s="3"/>
+      <c r="J66" s="2"/>
+      <c r="K66" s="2"/>
+      <c r="L66" s="3"/>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A67" s="2"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
+      <c r="H67" s="2"/>
+      <c r="I67" s="3"/>
+      <c r="J67" s="2"/>
+      <c r="K67" s="2"/>
+      <c r="L67" s="3"/>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A68" s="2"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+      <c r="I68" s="3"/>
+      <c r="J68" s="2"/>
+      <c r="K68" s="2"/>
+      <c r="L68" s="3"/>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A69" s="2"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="2"/>
+      <c r="I69" s="3"/>
+      <c r="J69" s="2"/>
+      <c r="K69" s="2"/>
+      <c r="L69" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>